<commit_message>
remove a year of data in the template
</commit_message>
<xml_diff>
--- a/RCaN/inst/extdata/CaN_template_mini.xlsx
+++ b/RCaN/inst/extdata/CaN_template_mini.xlsx
@@ -657,7 +657,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="153" zoomScaleNormal="153" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -883,47 +883,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1992</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>26816</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>7008</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>105000</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>7232</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>2976</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>560</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>68.568</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>1271.204</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>588.49</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>5.97415</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>1000000</v>
-      </c>
-    </row>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
remove initial biomass in the template
</commit_message>
<xml_diff>
--- a/RCaN/inst/extdata/CaN_template_mini.xlsx
+++ b/RCaN/inst/extdata/CaN_template_mini.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t xml:space="preserve">Template for input data to CaN models</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">in_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialBiomass</t>
   </si>
   <si>
     <t xml:space="preserve">AssimilationE</t>
@@ -314,7 +311,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="H3:H4 D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,18 +415,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>16</v>
       </c>
@@ -454,87 +452,76 @@
       <c r="H1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="n">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>166.08</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>16608</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>0.9</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <f aca="false">ROUND(C3/100,3)</f>
-        <v>166.08</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="E4" s="0" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>168.64</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>16864</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <f aca="false">ROUND(C4/100,3)</f>
-        <v>168.64</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -556,7 +543,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="189" zoomScaleNormal="189" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="H3:H4 B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -566,27 +553,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -595,13 +582,13 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -610,13 +597,13 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -625,13 +612,13 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -656,8 +643,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="153" zoomScaleNormal="153" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="153" zoomScaleNormal="153" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="H3:H4 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,43 +667,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +911,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="215" zoomScaleNormal="215" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="H3:H4 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -936,46 +923,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mmise à jour du template pour prise en compte contrainte active ou non
</commit_message>
<xml_diff>
--- a/RCaN/inst/extdata/CaN_template_mini.xlsx
+++ b/RCaN/inst/extdata/CaN_template_mini.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t xml:space="preserve">Template for input data to CaN models</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Time-range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
   </si>
   <si>
     <t xml:space="preserve">C01</t>
@@ -311,7 +314,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="H3:H4 D13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,8 +420,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,7 +546,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="189" zoomScaleNormal="189" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="H3:H4 B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -644,7 +647,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="153" zoomScaleNormal="153" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="H3:H4 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -908,10 +911,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="215" zoomScaleNormal="215" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="H3:H4 B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="215" zoomScaleNormal="215" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,38 +934,50 @@
       <c r="C1" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>56</v>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all data is 0 in 1 for boolean
</commit_message>
<xml_diff>
--- a/RCaN/inst/extdata/CaN_template_mini.xlsx
+++ b/RCaN/inst/extdata/CaN_template_mini.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t xml:space="preserve">Template for input data to CaN models</t>
   </si>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Component</t>
   </si>
   <si>
-    <t xml:space="preserve">in_out</t>
+    <t xml:space="preserve">Inside</t>
   </si>
   <si>
     <t xml:space="preserve">AssimilationE</t>
@@ -101,13 +101,7 @@
     <t xml:space="preserve">PhytoAndBacteria</t>
   </si>
   <si>
-    <t xml:space="preserve">Out</t>
-  </si>
-  <si>
     <t xml:space="preserve">HerbZooplankton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In</t>
   </si>
   <si>
     <t xml:space="preserve">OmniZooplankton</t>
@@ -296,18 +290,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -317,10 +311,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -414,20 +405,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,8 +450,8 @@
       <c r="A2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>25</v>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.65</v>
@@ -469,10 +459,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -495,10 +485,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -521,10 +511,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -549,34 +539,31 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -585,13 +572,13 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -600,13 +587,13 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -615,13 +602,13 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -640,7 +627,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -650,7 +637,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.34"/>
@@ -661,52 +648,51 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,46 +893,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="215" zoomScaleNormal="215" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="215" zoomScaleNormal="215" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -954,13 +938,13 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -968,13 +952,13 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>

</xml_diff>